<commit_message>
Update code to check if assigned lecturer id != null then assin lecturer for better performance
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/Book1.xlsx
+++ b/TeachingAssignmentManagement/Uploads/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A430997-ECF2-4ADA-B26E-741867FD25DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C7B9C7-6FEC-4CEB-BCAC-164FCC20D9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA9049D4-CE1C-430B-B4D2-1DC9BD9BDC48}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{280A5DBE-2C58-4381-8812-4F94F06631ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,108 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="109">
-  <si>
-    <t>MaGocLHP</t>
-  </si>
-  <si>
-    <t>Mã MH</t>
-  </si>
-  <si>
-    <t>Mã LHP</t>
-  </si>
-  <si>
-    <t>Tên HP</t>
-  </si>
-  <si>
-    <t>Số TC</t>
-  </si>
-  <si>
-    <t>Loại HP</t>
-  </si>
-  <si>
-    <t>Mã Lớp</t>
-  </si>
-  <si>
-    <t>TSMH</t>
-  </si>
-  <si>
-    <t>Số Tiết Đã xếp</t>
-  </si>
-  <si>
-    <t>PH</t>
-  </si>
-  <si>
-    <t>Thứ</t>
-  </si>
-  <si>
-    <t>Tiết BĐ</t>
-  </si>
-  <si>
-    <t>Số Tiết</t>
-  </si>
-  <si>
-    <t>Tiết Học</t>
-  </si>
-  <si>
-    <t>Phòng</t>
-  </si>
-  <si>
-    <t>Mã CBGD</t>
-  </si>
-  <si>
-    <t>Tên CBGD</t>
-  </si>
-  <si>
-    <t>PH_X</t>
-  </si>
-  <si>
-    <t>Sức Chứa</t>
-  </si>
-  <si>
-    <t>SiSoTKB</t>
-  </si>
-  <si>
-    <t>Trống</t>
-  </si>
-  <si>
-    <t>Tình Trạng LHP</t>
-  </si>
-  <si>
-    <t>TuanHoc2</t>
-  </si>
-  <si>
-    <t>ThuS</t>
-  </si>
-  <si>
-    <t>TietS</t>
-  </si>
-  <si>
-    <t>Số SVĐK</t>
-  </si>
-  <si>
-    <t>Tuần BD</t>
-  </si>
-  <si>
-    <t>Tuần KT</t>
-  </si>
-  <si>
-    <t>Ghi Chú 1</t>
-  </si>
-  <si>
-    <t>Ghi chú 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="112">
   <si>
     <t>223_71ITSE30503_0103</t>
   </si>
   <si>
-    <t>71ITSE30503</t>
-  </si>
-  <si>
     <t>Lập trình ứng dụng Web</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>Thực hành</t>
@@ -162,58 +66,28 @@
 71K27CNT</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Thứ Sáu</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>7 - 9</t>
-  </si>
-  <si>
     <t>CS2.C.04.08</t>
   </si>
   <si>
+    <t>Võ Anh Tiến</t>
+  </si>
+  <si>
     <t>PMT</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>-2</t>
-  </si>
-  <si>
     <t>Ngừng đăng ký qua mạng</t>
   </si>
   <si>
     <t>37,38,39,40,41,42,43,44,45,46</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>7480201</t>
-  </si>
-  <si>
     <t>Công nghệ thông tin</t>
   </si>
   <si>
     <t>223_71ITSE30603_0101</t>
-  </si>
-  <si>
-    <t>71ITSE30603</t>
   </si>
   <si>
     <t>Lập trình ứng dụng di động</t>
@@ -238,19 +112,10 @@
 71K27CNT</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
     <t>Thứ Bảy</t>
   </si>
   <si>
     <t>CS3.F.12.05</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>-4</t>
   </si>
   <si>
     <t>223_71ITSE30603_0102</t>
@@ -275,15 +140,6 @@
 71K27CNT</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>10 - 12</t>
-  </si>
-  <si>
-    <t>-3</t>
-  </si>
-  <si>
     <t>223_71ITSE30603_0203</t>
   </si>
   <si>
@@ -312,13 +168,7 @@
     <t>CS3.F.12.07</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>223_71ITSE30903_0102</t>
-  </si>
-  <si>
-    <t>71ITSE30903</t>
   </si>
   <si>
     <t>Thiết kế giao diện người dùng</t>
@@ -346,15 +196,6 @@
     <t>Thứ Tư</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>223_71ITSE30903_0103</t>
   </si>
   <si>
@@ -377,9 +218,6 @@
 71K27CNT</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>13 - 15</t>
   </si>
   <si>
@@ -411,9 +249,6 @@
     <t>Thứ Năm</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>223_71ITSE30903_0301</t>
   </si>
   <si>
@@ -467,53 +302,227 @@
     <t>CS3.G.08.29</t>
   </si>
   <si>
+    <t>222_DIT0330_0102</t>
+  </si>
+  <si>
+    <t>Thương mại điện tử và mạng xã hội</t>
+  </si>
+  <si>
+    <t>K25T-IT1, K25T-IT10, K25T-IT11, K25T-IT12, K25T-IT13, K25T-IT14, K25T-IT15, K25T-IT16, K25T-IT17, K25T-IT2, K25T-IT3, K25T-IT4, K25T-IT5, K25T-IT6, K25T-IT7, K25T-IT8, K25T-IT9</t>
+  </si>
+  <si>
+    <t>CS3.F.12.02</t>
+  </si>
+  <si>
+    <t>Được chấp nhận</t>
+  </si>
+  <si>
+    <t>32,33,34,35,36,37,38,39,40,41</t>
+  </si>
+  <si>
+    <t>222_DIT0330_0201</t>
+  </si>
+  <si>
+    <t>Mã LHP</t>
+  </si>
+  <si>
+    <t>Tên HP</t>
+  </si>
+  <si>
+    <t>Số TC</t>
+  </si>
+  <si>
+    <t>Loại HP</t>
+  </si>
+  <si>
+    <t>Mã Lớp</t>
+  </si>
+  <si>
+    <t>TSMH</t>
+  </si>
+  <si>
+    <t>Số Tiết Đã xếp</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>Thứ</t>
+  </si>
+  <si>
+    <t>Tiết BĐ</t>
+  </si>
+  <si>
+    <t>Số Tiết</t>
+  </si>
+  <si>
+    <t>Tiết Học</t>
+  </si>
+  <si>
+    <t>Phòng</t>
+  </si>
+  <si>
+    <t>Mã CBGD</t>
+  </si>
+  <si>
+    <t>Tên CBGD</t>
+  </si>
+  <si>
+    <t>PH_X</t>
+  </si>
+  <si>
+    <t>Sức Chứa</t>
+  </si>
+  <si>
+    <t>SiSoTKB</t>
+  </si>
+  <si>
+    <t>Trống</t>
+  </si>
+  <si>
+    <t>Tình Trạng LHP</t>
+  </si>
+  <si>
+    <t>TuanHoc2</t>
+  </si>
+  <si>
+    <t>ThuS</t>
+  </si>
+  <si>
+    <t>TietS</t>
+  </si>
+  <si>
+    <t>Số SVĐK</t>
+  </si>
+  <si>
+    <t>Tuần BD</t>
+  </si>
+  <si>
+    <t>Tuần KT</t>
+  </si>
+  <si>
+    <t>Ghi Chú 1</t>
+  </si>
+  <si>
+    <t>Ghi chú 2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>7 - 9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10 - 12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>7480201</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
     <t>-1</t>
   </si>
   <si>
-    <t>222_DIT0330_0102</t>
+    <t>34</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>2001102245</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>MaGocLHP</t>
+  </si>
+  <si>
+    <t>Mã MH</t>
+  </si>
+  <si>
+    <t>71ITSE30503</t>
+  </si>
+  <si>
+    <t>71ITSE30603</t>
+  </si>
+  <si>
+    <t>71ITSE30903</t>
   </si>
   <si>
     <t>DIT0330</t>
   </si>
   <si>
-    <t>Thương mại điện tử và mạng xã hội</t>
-  </si>
-  <si>
-    <t>K25T-IT1, K25T-IT10, K25T-IT11, K25T-IT12, K25T-IT13, K25T-IT14, K25T-IT15, K25T-IT16, K25T-IT17, K25T-IT2, K25T-IT3, K25T-IT4, K25T-IT5, K25T-IT6, K25T-IT7, K25T-IT8, K25T-IT9</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>CS3.F.12.02</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Được chấp nhận</t>
-  </si>
-  <si>
-    <t>32,33,34,35,36,37,38,39,40,41</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>222_DIT0330_0201</t>
-  </si>
-  <si>
-    <t>15</t>
+    <t>Chủ Nhật</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,13 +537,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -873,1058 +875,1265 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E77AA8-5061-42BF-9C57-1CC22A8FAAF2}">
-  <dimension ref="A1:AD12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EED5CF-5D3B-4B27-8BE4-7F2B1F392DFD}">
+  <dimension ref="A1:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="M2" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="N2" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="O2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2">
-        <v>2001102245</v>
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>6</v>
       </c>
       <c r="R2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="S2" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="T2" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="U2" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="V2" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="W2" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="X2" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="Y2" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="Z2" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="AA2" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AB2" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="AC2" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD2" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="K3" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="O3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3">
-        <v>2001102245</v>
+        <v>15</v>
+      </c>
+      <c r="P3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>6</v>
       </c>
       <c r="R3" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="S3" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="T3" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="U3" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="V3" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="W3" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="X3" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="Y3" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="Z3" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AA3" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AB3" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="AC3" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD3" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="N4" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="O4" t="s">
-        <v>58</v>
-      </c>
-      <c r="P4">
-        <v>2001102245</v>
+        <v>15</v>
+      </c>
+      <c r="P4" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>6</v>
       </c>
       <c r="R4" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="S4" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="U4" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="V4" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="W4" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="X4" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="Y4" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="Z4" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AA4" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AB4" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="AC4" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD4" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="O5" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5">
-        <v>2001102245</v>
+        <v>21</v>
+      </c>
+      <c r="P5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>6</v>
       </c>
       <c r="R5" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="S5" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="U5" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="V5" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="W5" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="X5" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="Y5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="Z5" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AA5" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AB5" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="AC5" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD5" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="K6" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="M6" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="N6" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="O6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P6">
-        <v>2001102245</v>
+        <v>21</v>
+      </c>
+      <c r="P6" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>6</v>
       </c>
       <c r="R6" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="S6" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="T6" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="U6" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="V6" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="W6" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="X6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Y6" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="Z6" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AA6" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AB6" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="AC6" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD6" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" t="s">
+        <v>7</v>
+      </c>
+      <c r="S7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T7" t="s">
+        <v>86</v>
+      </c>
+      <c r="U7" t="s">
+        <v>96</v>
+      </c>
+      <c r="V7" t="s">
+        <v>8</v>
+      </c>
+      <c r="W7" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" t="s">
         <v>79</v>
       </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" t="s">
-        <v>81</v>
-      </c>
-      <c r="M7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" t="s">
-        <v>82</v>
-      </c>
-      <c r="O7" t="s">
-        <v>83</v>
-      </c>
-      <c r="P7">
-        <v>2001102245</v>
-      </c>
-      <c r="R7" t="s">
-        <v>41</v>
-      </c>
-      <c r="S7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U7" t="s">
-        <v>76</v>
-      </c>
-      <c r="V7" t="s">
-        <v>45</v>
-      </c>
-      <c r="W7" t="s">
-        <v>46</v>
-      </c>
-      <c r="X7" t="s">
-        <v>77</v>
-      </c>
       <c r="Y7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="Z7" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="AA7" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AB7" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="AC7" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD7" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
         <v>85</v>
       </c>
-      <c r="H8" t="s">
-        <v>56</v>
-      </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="K8" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="M8" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="N8" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="O8" t="s">
-        <v>69</v>
-      </c>
-      <c r="P8">
-        <v>2001102245</v>
+        <v>21</v>
+      </c>
+      <c r="P8" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>6</v>
       </c>
       <c r="R8" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="S8" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="T8" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="U8" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="V8" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="W8" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="X8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z8" t="s">
         <v>87</v>
       </c>
-      <c r="Y8" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>59</v>
-      </c>
       <c r="AA8" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="AB8" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="AC8" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD8" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" t="s">
+        <v>82</v>
+      </c>
+      <c r="M9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" t="s">
+        <v>83</v>
+      </c>
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" t="s">
+        <v>7</v>
+      </c>
+      <c r="S9" t="s">
+        <v>87</v>
+      </c>
+      <c r="T9" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" t="s">
+        <v>96</v>
+      </c>
+      <c r="V9" t="s">
+        <v>8</v>
+      </c>
+      <c r="W9" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC9" t="s">
         <v>88</v>
       </c>
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M9" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" t="s">
-        <v>64</v>
-      </c>
-      <c r="O9" t="s">
-        <v>90</v>
-      </c>
-      <c r="P9">
-        <v>2001102245</v>
-      </c>
-      <c r="R9" t="s">
-        <v>41</v>
-      </c>
-      <c r="S9" t="s">
-        <v>59</v>
-      </c>
-      <c r="T9" t="s">
-        <v>59</v>
-      </c>
-      <c r="U9" t="s">
-        <v>76</v>
-      </c>
-      <c r="V9" t="s">
-        <v>45</v>
-      </c>
-      <c r="W9" t="s">
-        <v>46</v>
-      </c>
-      <c r="X9" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>50</v>
-      </c>
       <c r="AD9" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" t="s">
+        <v>83</v>
+      </c>
+      <c r="O10" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" t="s">
+        <v>7</v>
+      </c>
+      <c r="S10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T10" t="s">
+        <v>87</v>
+      </c>
+      <c r="U10" t="s">
+        <v>94</v>
+      </c>
+      <c r="V10" t="s">
+        <v>8</v>
+      </c>
+      <c r="W10" t="s">
+        <v>9</v>
+      </c>
+      <c r="X10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA10" t="s">
         <v>92</v>
       </c>
-      <c r="H10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="AB10" t="s">
         <v>93</v>
       </c>
-      <c r="L10" t="s">
-        <v>63</v>
-      </c>
-      <c r="M10" t="s">
-        <v>33</v>
-      </c>
-      <c r="N10" t="s">
-        <v>64</v>
-      </c>
-      <c r="O10" t="s">
-        <v>94</v>
-      </c>
-      <c r="P10">
-        <v>2001102245</v>
-      </c>
-      <c r="R10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S10" t="s">
-        <v>78</v>
-      </c>
-      <c r="T10" t="s">
-        <v>59</v>
-      </c>
-      <c r="U10" t="s">
-        <v>95</v>
-      </c>
-      <c r="V10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>49</v>
-      </c>
       <c r="AC10" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD10" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="L11" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="M11" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="N11" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="O11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P11" t="s">
         <v>101</v>
       </c>
-      <c r="P11">
-        <v>2001102245</v>
+      <c r="Q11" t="s">
+        <v>6</v>
       </c>
       <c r="R11" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="S11" t="s">
+        <v>91</v>
+      </c>
+      <c r="T11" t="s">
+        <v>86</v>
+      </c>
+      <c r="U11" t="s">
+        <v>95</v>
+      </c>
+      <c r="V11" t="s">
+        <v>44</v>
+      </c>
+      <c r="W11" t="s">
+        <v>45</v>
+      </c>
+      <c r="X11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB11" t="s">
         <v>102</v>
       </c>
-      <c r="T11" t="s">
-        <v>36</v>
-      </c>
-      <c r="U11" t="s">
-        <v>103</v>
-      </c>
-      <c r="V11" t="s">
-        <v>104</v>
-      </c>
-      <c r="W11" t="s">
-        <v>105</v>
-      </c>
-      <c r="X11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>106</v>
-      </c>
       <c r="AC11" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="AD11" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="I12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="M12" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="N12" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="O12" t="s">
-        <v>90</v>
-      </c>
-      <c r="P12">
-        <v>2001102245</v>
+        <v>35</v>
+      </c>
+      <c r="P12" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>6</v>
       </c>
       <c r="R12" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12" t="s">
+        <v>87</v>
+      </c>
+      <c r="T12" t="s">
+        <v>86</v>
+      </c>
+      <c r="U12" t="s">
+        <v>75</v>
+      </c>
+      <c r="V12" t="s">
+        <v>44</v>
+      </c>
+      <c r="W12" t="s">
+        <v>45</v>
+      </c>
+      <c r="X12" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
         <v>41</v>
       </c>
-      <c r="S12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T12" t="s">
-        <v>36</v>
-      </c>
-      <c r="U12" t="s">
-        <v>33</v>
-      </c>
-      <c r="V12" t="s">
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" t="s">
         <v>104</v>
       </c>
-      <c r="W12" t="s">
-        <v>105</v>
-      </c>
-      <c r="X12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB12" t="s">
+      <c r="K13" t="s">
+        <v>111</v>
+      </c>
+      <c r="L13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M13" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" t="s">
+        <v>83</v>
+      </c>
+      <c r="O13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P13" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" t="s">
+        <v>7</v>
+      </c>
+      <c r="S13" t="s">
+        <v>87</v>
+      </c>
+      <c r="T13" t="s">
+        <v>86</v>
+      </c>
+      <c r="U13" t="s">
+        <v>75</v>
+      </c>
+      <c r="V13" t="s">
+        <v>44</v>
+      </c>
+      <c r="W13" t="s">
+        <v>45</v>
+      </c>
+      <c r="X13">
+        <v>8</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
         <v>42</v>
       </c>
-      <c r="AC12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>51</v>
+      <c r="H14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" t="s">
+        <v>82</v>
+      </c>
+      <c r="M14" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" t="s">
+        <v>83</v>
+      </c>
+      <c r="O14" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>6</v>
+      </c>
+      <c r="R14" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14" t="s">
+        <v>87</v>
+      </c>
+      <c r="T14" t="s">
+        <v>86</v>
+      </c>
+      <c r="U14" t="s">
+        <v>75</v>
+      </c>
+      <c r="V14" t="s">
+        <v>44</v>
+      </c>
+      <c r="W14" t="s">
+        <v>45</v>
+      </c>
+      <c r="X14">
+        <v>2</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>